<commit_message>
Fixed a typo in the `OrderResponse` document type of "PEPPOL Ordering profile V1"
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$E$30</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Common Name</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::Order##urn:www.cenbii.eu:transaction:biitrns076:ver2.0:extended:urn:www.peppol.eu:bis:peppol28a:ver1.0:extended:urn:fdc:peppol-authority.co.uk:spec:ordering:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:www.cenbii.eu:transaction:biitrns076:ver2.0:extended:urn:www.peppol.eu:bis:peppol28a:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>Typo in name!</t>
   </si>
 </sst>
 </file>
@@ -706,11 +712,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,8 +725,9 @@
     <col min="2" max="2" width="132.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -998,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -1013,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
@@ -1043,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -1088,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>41</v>
       </c>
@@ -1103,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
@@ -1136,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -1151,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
@@ -1162,31 +1169,36 @@
         <v>31</v>
       </c>
       <c r="D27" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3</v>
+      </c>
+      <c r="D28" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>31</v>
@@ -1196,45 +1208,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>56</v>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="6">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="D30" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6">
+        <v>2</v>
+      </c>
+      <c r="D31" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="6">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="8">
-        <v>3</v>
+      <c r="C32" s="6">
+        <v>2</v>
       </c>
       <c r="D32" s="6" t="b">
         <f>FALSE</f>
@@ -1243,10 +1255,10 @@
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="8">
         <v>3</v>
@@ -1256,8 +1268,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3</v>
+      </c>
+      <c r="D34" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E29"/>
+  <autoFilter ref="A1:E30"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C13:C15" twoDigitTextYear="1"/>

</xml_diff>

<commit_message>
Added BIS Billing V3 CII binding
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Common Name</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Typo in name!</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::D16B</t>
   </si>
 </sst>
 </file>
@@ -712,11 +715,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,6 +1286,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="6">
+        <v>3</v>
+      </c>
+      <c r="D35" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E30"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added PrAcc document type Ids
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
   <si>
     <t>Common Name</t>
   </si>
@@ -217,6 +217,33 @@
   </si>
   <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::D16B</t>
+  </si>
+  <si>
+    <t>Procurement procedure subscription V1</t>
+  </si>
+  <si>
+    <t>Procurement document access V1</t>
+  </si>
+  <si>
+    <t>Tender Submission V1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:ExpressionOfInterestRequest-2::ExpressionOfInterestRequest##urn:www.cenbii.eu:transaction:biitrdm081:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t001:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:ExpressionOfInterestResponse-2::ExpressionOfInterestResponse##urn:www.cenbii.eu:transaction:biitrdm082:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t002:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:TenderStatusRequest-2::TenderStatusRequest##urn:www.cenbii.eu:transaction:biitrdm097:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t003:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CallForTenders-2::CallForTenders##urn:www.cenbii.eu:transaction:biitrdm083:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t004:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:TenderReceipt-2::TenderReceipt##urn:www.cenbii.eu:transaction:biitrdm045:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t006:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Tender-2::Tender##urn:www.cenbii.eu:transaction:biitrdm090:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t005:ver1.0::2.2</t>
   </si>
 </sst>
 </file>
@@ -282,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -309,6 +336,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -715,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,6 +1331,96 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="6">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="6">
+        <v>3</v>
+      </c>
+      <c r="D37" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="6">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="6">
+        <v>3</v>
+      </c>
+      <c r="D39" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="6">
+        <v>3</v>
+      </c>
+      <c r="D40" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="6">
+        <v>3</v>
+      </c>
+      <c r="D41" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E30"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed a typo in the `PEPPOL Order profile V2` document type. Correct: `peppol3a`. Old and invalid: `peppol03a`.
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -129,9 +129,6 @@
     <t>PEPPOL Order profile V2</t>
   </si>
   <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol03a:ver2.0::2.1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:www.cenbii.eu:transaction:biitrns010:ver2.0:extended:urn:www.peppol.eu:bis:peppol4a:ver2.0::2.1</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Tender-2::Tender##urn:www.cenbii.eu:transaction:biitrdm090:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t005:ver1.0::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol3a:ver2.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,10 +774,10 @@
         <v>18</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -890,10 +890,10 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>31</v>
@@ -926,7 +926,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>31</v>
@@ -959,7 +959,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>31</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>21</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>31</v>
@@ -1040,10 +1040,10 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>31</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>6</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>25</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>27</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>31</v>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>31</v>
@@ -1208,15 +1208,15 @@
         <v>3</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="8">
         <v>3</v>
@@ -1228,10 +1228,10 @@
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>31</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>31</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="6">
         <v>2</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="8">
         <v>3</v>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="8">
         <v>3</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="6">
         <v>3</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="6">
         <v>3</v>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="6">
         <v>3</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="6">
         <v>3</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="6">
         <v>3</v>
@@ -1393,10 +1393,10 @@
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" s="6">
         <v>3</v>
@@ -1408,10 +1408,10 @@
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="6">
         <v>3</v>

</xml_diff>

<commit_message>
Added `XRechnung Invoice V1.1` and `XRechnung CreditNote V1.1` document types (as EN 16931 CIUSes)
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$E$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$F$30</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn4" localSheetId="0">'Document Type'!#REF!</definedName>
-    <definedName name="_ftnref1" localSheetId="0">'Document Type'!$B$1</definedName>
+    <definedName name="_ftnref1" localSheetId="0">'Document Type'!$C$1</definedName>
     <definedName name="_ftnref2" localSheetId="0">'Document Type'!$A$2</definedName>
     <definedName name="_ftnref3" localSheetId="0">'Document Type'!$A$3</definedName>
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!$A$4</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
   <si>
     <t>Common Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>urn:www.peppol.eu:schema:xsd:CatalogueTemplate-1::CatalogueTemplate##urn:www.cenbii.eu:transaction:biicoretrdm993:ver0.1:#urn:www.peppol.eu:bis:peppol993a:ver1.0::0.1</t>
   </si>
   <si>
-    <t>PEPPOL Document Identifier</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biicoretrdm001:ver1.0:#urn:www.peppol.eu:bis:peppol3a:ver1.0::2.0</t>
   </si>
   <si>
@@ -244,6 +241,30 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol3a:ver2.0::2.1</t>
+  </si>
+  <si>
+    <t>PEPPOL Identifier Scheme</t>
+  </si>
+  <si>
+    <t>PEPPOL Document Type Identifier</t>
+  </si>
+  <si>
+    <t>busdox-docid-qns</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant# urn:xoev-de:kosit:standard:xrechnung_1.1::D16B</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
+  </si>
+  <si>
+    <t>XRechnung Invoice V1.1</t>
+  </si>
+  <si>
+    <t>XRechnung CreditNote V1.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
   </si>
 </sst>
 </file>
@@ -745,687 +766,865 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="132.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="132.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="6" t="b">
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="b">
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="6" t="b">
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6" t="b">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="6" t="b">
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="b">
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6" t="b">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6" t="b">
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="6" t="b">
+      <c r="D13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="6" t="b">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="6" t="b">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="6" t="b">
+      <c r="E24" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="D27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="8">
+        <v>3</v>
+      </c>
+      <c r="E28" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="B29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="8">
         <v>3</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="E33" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="8">
+        <v>3</v>
+      </c>
+      <c r="E34" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="8">
+      <c r="D35" s="6">
         <v>3</v>
       </c>
-      <c r="D28" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="6">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="6">
-        <v>2</v>
-      </c>
-      <c r="D32" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="E35" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="6">
         <v>3</v>
       </c>
-      <c r="D33" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="E36" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="6">
         <v>3</v>
       </c>
-      <c r="D34" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="6">
+      <c r="E37" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="6">
         <v>3</v>
       </c>
-      <c r="D35" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="E38" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="6">
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="6">
         <v>3</v>
       </c>
-      <c r="D36" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="6">
+      <c r="E39" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="6">
         <v>3</v>
       </c>
-      <c r="D37" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="E40" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="6">
+      <c r="B41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="6">
         <v>3</v>
       </c>
-      <c r="D38" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="6">
+      <c r="E41" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="10">
         <v>3</v>
       </c>
-      <c r="D39" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="E42" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="10">
         <v>3</v>
       </c>
-      <c r="D40" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="6">
+      <c r="E43" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="10">
         <v>3</v>
       </c>
-      <c r="D41" s="10" t="b">
+      <c r="E44" s="10" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E30"/>
+  <autoFilter ref="A1:F30"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C13:C15" twoDigitTextYear="1"/>
+    <ignoredError sqref="D13:D15" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added UBL.BE document types (TICC-54)
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v3.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
-  <si>
-    <t>Common Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -277,6 +274,21 @@
   </si>
   <si>
     <t>OIOUBL Reminder V2.02</t>
+  </si>
+  <si>
+    <t>UBL.BE Invoice 3.0</t>
+  </si>
+  <si>
+    <t>UBL.BE Credit Note 3.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:UBL.BE:1.0.0.20180214::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:UBL.BE:1.0.0.20180214::2.1</t>
+  </si>
+  <si>
+    <t>Profile code</t>
   </si>
 </sst>
 </file>
@@ -778,11 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,36 +811,36 @@
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="b">
         <f>TRUE</f>
@@ -840,16 +852,16 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="6" t="b">
         <f>TRUE</f>
@@ -861,16 +873,16 @@
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6" t="b">
         <f>TRUE</f>
@@ -882,16 +894,16 @@
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6" t="b">
         <f>TRUE</f>
@@ -903,16 +915,16 @@
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="b">
         <f>TRUE</f>
@@ -924,16 +936,16 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="b">
         <f>TRUE</f>
@@ -945,16 +957,16 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6" t="b">
         <f>FALSE</f>
@@ -963,16 +975,16 @@
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="b">
         <f>TRUE</f>
@@ -984,16 +996,16 @@
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="6" t="b">
         <f>FALSE</f>
@@ -1002,16 +1014,16 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6" t="b">
         <f>TRUE</f>
@@ -1023,16 +1035,16 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="6" t="b">
         <f>FALSE</f>
@@ -1041,16 +1053,16 @@
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="6" t="b">
         <f>TRUE</f>
@@ -1062,16 +1074,16 @@
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="6" t="b">
         <f>TRUE</f>
@@ -1083,16 +1095,16 @@
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="6" t="b">
         <f>TRUE</f>
@@ -1104,16 +1116,16 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D16" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="6" t="b">
         <f>FALSE</f>
@@ -1122,16 +1134,16 @@
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="6" t="b">
         <f>FALSE</f>
@@ -1140,16 +1152,16 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="6" t="b">
         <f>FALSE</f>
@@ -1158,16 +1170,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="6" t="b">
         <f>FALSE</f>
@@ -1176,16 +1188,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="6" t="b">
         <f>FALSE</f>
@@ -1194,16 +1206,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="6" t="b">
         <f>FALSE</f>
@@ -1212,16 +1224,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="6" t="b">
         <f>FALSE</f>
@@ -1230,16 +1242,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="6" t="b">
         <f>FALSE</f>
@@ -1248,16 +1260,16 @@
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E24" s="6" t="b">
         <f>TRUE</f>
@@ -1269,16 +1281,16 @@
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="6" t="b">
         <f>FALSE</f>
@@ -1287,16 +1299,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="6" t="b">
         <f>FALSE</f>
@@ -1305,16 +1317,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" s="6" t="b">
         <v>1</v>
@@ -1323,18 +1335,18 @@
         <v>3</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" s="8">
         <v>3</v>
@@ -1346,16 +1358,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" s="6" t="b">
         <f>FALSE</f>
@@ -1364,16 +1376,16 @@
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E30" s="6" t="b">
         <f>FALSE</f>
@@ -1382,13 +1394,13 @@
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="6">
         <v>2</v>
@@ -1400,13 +1412,13 @@
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="6">
         <v>2</v>
@@ -1418,13 +1430,13 @@
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="8">
         <v>3</v>
@@ -1436,13 +1448,13 @@
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1454,13 +1466,13 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="6">
         <v>3</v>
@@ -1472,13 +1484,13 @@
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -1490,13 +1502,13 @@
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -1508,13 +1520,13 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -1526,13 +1538,13 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1544,13 +1556,13 @@
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1562,13 +1574,13 @@
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1580,13 +1592,13 @@
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="10">
         <v>3</v>
@@ -1598,13 +1610,13 @@
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1616,13 +1628,13 @@
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1634,13 +1646,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1652,18 +1664,54 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="10">
+        <v>3</v>
+      </c>
+      <c r="E46" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="10">
-        <v>3</v>
-      </c>
-      <c r="E46" s="10" t="b">
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="10">
+        <v>3</v>
+      </c>
+      <c r="E47" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="10">
+        <v>3</v>
+      </c>
+      <c r="E48" s="10" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>

</xml_diff>